<commit_message>
se adiciona refactorizacion de unidad 3
</commit_message>
<xml_diff>
--- a/src/test/resources/dataprueba/dataPrueba.xlsx
+++ b/src/test/resources/dataprueba/dataPrueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/estebanhontavillaantich/IntroSelenium/src/test/resources/dataprueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F12474-7FA3-EC45-9240-8C631215B98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653CBE2-3090-9449-B869-B2ACE32E4E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{76037C72-AC24-4F08-916C-0EBDA7347AF8}"/>
   </bookViews>
@@ -205,10 +205,10 @@
 No customer account found</t>
   </si>
   <si>
-    <t>esantich@gmailis.com</t>
-  </si>
-  <si>
-    <t>este@jemaili.com</t>
+    <t>estaantich@gmailis.com</t>
+  </si>
+  <si>
+    <t>esteb@jemaili.com</t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A645B1A7-99A1-40F5-8614-AC97BD27FDDC}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>